<commit_message>
seperate download and save complete
</commit_message>
<xml_diff>
--- a/public/Work Activities_hyunmyung.kim.xlsx
+++ b/public/Work Activities_hyunmyung.kim.xlsx
@@ -1,30 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966CC15B-5B9F-4EA0-9C9D-2C071A8FF7B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Daily Report" sheetId="135" r:id="rId1"/>
+    <sheet sheetId="135" name="Daily Report" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Daily Report'!$A1:$G31</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -37,7 +25,7 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>ARMC Door Replace Phase 1</t>
+    <t>Health Center - Icardo Plaza ADA Improvements and Road Repairs</t>
   </si>
   <si>
     <t>DATE</t>
@@ -49,7 +37,7 @@
     <t>CONTRACT NO.</t>
   </si>
   <si>
-    <t>19-824-10.10.0851-02</t>
+    <t>TOCA3866C-09.00</t>
   </si>
   <si>
     <t xml:space="preserve">PROJECT ID </t>
@@ -91,7 +79,7 @@
     <t>NO. OF WORKERS</t>
   </si>
   <si>
-    <t>HOURS
+    <t xml:space="preserve">HOURS
 /Day</t>
   </si>
   <si>
@@ -110,44 +98,44 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm AM/PM;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="20"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <family val="2"/>
+      <scheme val="minor"/>
       <sz val="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -165,7 +153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -693,33 +681,105 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -735,6 +795,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -750,173 +816,89 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -937,7 +919,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:oneCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
@@ -947,7 +929,7 @@
     <xdr:ext cx="1476375" cy="428625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="1" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -1298,15 +1280,13 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N37"/>
+<file path=xl/worksheets/sheet135.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
@@ -1316,425 +1296,469 @@
     <col min="6" max="6" width="15.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="16384" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" ht="48.75" customHeight="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" ht="19.5" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="37"/>
-    </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" ht="19.5" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="36">
-        <v>6133</v>
-      </c>
-      <c r="G3" s="37"/>
-    </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="F3" s="13">
+        <v>6141</v>
+      </c>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" ht="19.5" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="8" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="42"/>
-    </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" ht="19.5" customHeight="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="8" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="42"/>
-    </row>
-    <row r="6" spans="1:14" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="53" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="F6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="46"/>
-    </row>
-    <row r="7" spans="1:14" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="11" t="s">
+      <c r="G6" s="30"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="54"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48"/>
-    </row>
-    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56"/>
-    </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="58"/>
-      <c r="M9" s="23"/>
-    </row>
-    <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="58"/>
-    </row>
-    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
-    </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
-    </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="58"/>
-    </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58"/>
-    </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-    </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
+    </row>
+    <row r="8" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
+    </row>
+    <row r="9" ht="19.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
+      <c r="M9" s="51"/>
+    </row>
+    <row r="10" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+    </row>
+    <row r="11" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="44"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="50"/>
+    </row>
+    <row r="12" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="44"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="50"/>
+    </row>
+    <row r="13" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="44"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
+    </row>
+    <row r="14" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="44"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1" spans="1:16" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="24">
+      <c r="B16" s="53"/>
+      <c r="C16" s="54">
         <f>SUM(C8:C15)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="63"/>
-      <c r="N16" s="26"/>
-    </row>
-    <row r="17" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="64" t="s">
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="58"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+    </row>
+    <row r="17" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="66"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="67" t="s">
+    <row r="18" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="69"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="65"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="70"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="72"/>
+    <row r="19" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="66"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="70"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="72"/>
-    </row>
-    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="73"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="75"/>
-    </row>
-    <row r="22" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="64" t="s">
+    <row r="20" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="66"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="68"/>
+    </row>
+    <row r="21" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="69"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="71"/>
+    </row>
+    <row r="22" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="66"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="62"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="67" t="s">
+    <row r="23" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="69"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="70"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="72"/>
-    </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="70"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="72"/>
-    </row>
-    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="75"/>
-    </row>
-    <row r="27" spans="1:14" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="64" t="s">
+    <row r="24" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="66"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="68"/>
+    </row>
+    <row r="25" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="66"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="68"/>
+    </row>
+    <row r="26" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="71"/>
+    </row>
+    <row r="27" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="66"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="62"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="67" t="s">
+    <row r="28" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="69"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="65"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="70"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="72"/>
+    <row r="29" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="66"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="68"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="70"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="72"/>
+    <row r="30" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="66"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="76"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="27"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="28"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="27"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="28"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="27"/>
+    <row r="31" ht="18" customHeight="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="72"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="74"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="75"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="76"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="75"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="75"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="76"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="75"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A23:G26"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A28:G31"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A18:G21"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G7"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G21"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A23:G26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A28:G31"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
       <formula1>"Sunny, Cloudy, Partly Cloudy, Windy, Rainy, Foggy, Snowy"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.46" right="0.32" top="0.57999999999999996" bottom="0.45" header="0.56999999999999995" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageMargins left="0.46" right="0.32" top="0.58" bottom="0.45" header="0.57" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="0" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>